<commit_message>
feat: show overtime import errors
</commit_message>
<xml_diff>
--- a/AccuPay/ImportTemplates/accupay-overtime-template.xlsx
+++ b/AccuPay/ImportTemplates/accupay-overtime-template.xlsx
@@ -1,30 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView windowWidth="19890" windowHeight="8355"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6">
   <si>
     <t>EmployeeID</t>
   </si>
   <si>
-    <t>Name of allowance</t>
+    <t>Type</t>
   </si>
   <si>
     <t>Effective start date</t>
@@ -43,30 +38,373 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -74,25 +412,311 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
+    <cellStyle name="Comma" xfId="2" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
+    <cellStyle name="Currency" xfId="5" builtinId="4"/>
+    <cellStyle name="Percent" xfId="6" builtinId="5"/>
+    <cellStyle name="Check Cell" xfId="7" builtinId="23"/>
+    <cellStyle name="Heading 2" xfId="8" builtinId="17"/>
+    <cellStyle name="Note" xfId="9" builtinId="10"/>
+    <cellStyle name="Hyperlink" xfId="10" builtinId="8"/>
+    <cellStyle name="60% - Accent4" xfId="11" builtinId="44"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9"/>
+    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
+    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
+    <cellStyle name="Title" xfId="16" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
+    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
+    <cellStyle name="Input" xfId="21" builtinId="20"/>
+    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
+    <cellStyle name="Good" xfId="23" builtinId="26"/>
+    <cellStyle name="Output" xfId="24" builtinId="21"/>
+    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
+    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
+    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
+    <cellStyle name="Total" xfId="28" builtinId="25"/>
+    <cellStyle name="Bad" xfId="29" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
+    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
+    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
+    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
+    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
+    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
+    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -350,31 +974,26 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="5"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.7142857142857" customWidth="1"/>
+    <col min="2" max="2" width="18.2857142857143" customWidth="1"/>
+    <col min="3" max="3" width="18" customWidth="1"/>
+    <col min="4" max="4" width="18.5714285714286" customWidth="1"/>
+    <col min="5" max="5" width="17.4285714285714" customWidth="1"/>
+    <col min="6" max="6" width="17.7142857142857" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -398,6 +1017,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fix issues on import overtime caused by the recent changes.
</commit_message>
<xml_diff>
--- a/AccuPay/ImportTemplates/accupay-overtime-template.xlsx
+++ b/AccuPay/ImportTemplates/accupay-overtime-template.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t xml:space="preserve">EmployeeID</t>
   </si>
@@ -29,9 +29,6 @@
   </si>
   <si>
     <t xml:space="preserve">Effective Start Time</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Effective end date</t>
   </si>
   <si>
     <t xml:space="preserve">Effective End Time</t>
@@ -142,21 +139,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
+      <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.01171875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="18.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="17.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="17.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1023" min="6" style="0" width="9"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1024" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="17.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1023" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -172,9 +167,6 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
Resolve conflicts then merge branch 'master' into feature/laglobal.
</commit_message>
<xml_diff>
--- a/AccuPay/ImportTemplates/accupay-overtime-template.xlsx
+++ b/AccuPay/ImportTemplates/accupay-overtime-template.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t xml:space="preserve">EmployeeID</t>
   </si>
@@ -29,9 +29,6 @@
   </si>
   <si>
     <t xml:space="preserve">Effective Start Time</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Effective end date</t>
   </si>
   <si>
     <t xml:space="preserve">Effective End Time</t>
@@ -142,21 +139,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
+      <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.01171875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="18.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="17.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="17.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1023" min="6" style="0" width="9"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1024" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="17.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1023" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -172,9 +167,6 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
fix: overtime import open to all
</commit_message>
<xml_diff>
--- a/AccuPay/ImportTemplates/accupay-overtime-template.xlsx
+++ b/AccuPay/ImportTemplates/accupay-overtime-template.xlsx
@@ -8,6 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Lambert\accupay\AccuPay\ImportTemplates\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="InRGFyeJnvW3l1AQiD532wgjztNXWYPAb3468EBSkn+Hm+S80Kgx8nzuHdGkuxL95FX7cQAbZIotc2+sQpo+wg==" workbookSaltValue="grTQ5auLzl02Zd3Ybh4ySA==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
   </bookViews>
@@ -54,12 +55,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -87,11 +89,11 @@
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -375,41 +377,42 @@
   <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" style="4" customWidth="1"/>
-    <col min="2" max="2" width="18" style="4" customWidth="1"/>
-    <col min="3" max="3" width="18.5703125" style="4" customWidth="1"/>
-    <col min="4" max="4" width="17.7109375" style="4" customWidth="1"/>
-    <col min="5" max="5" width="0" style="3" hidden="1" customWidth="1"/>
-    <col min="6" max="1022" width="9" style="3"/>
-    <col min="1023" max="1025" width="11.5703125" style="3" customWidth="1"/>
-    <col min="1026" max="16384" width="9" style="3"/>
+    <col min="1" max="1" width="89.7109375" style="3" customWidth="1"/>
+    <col min="2" max="2" width="18" style="3" customWidth="1"/>
+    <col min="3" max="3" width="18.5703125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="17.7109375" style="3" customWidth="1"/>
+    <col min="5" max="5" width="0" style="2" hidden="1" customWidth="1"/>
+    <col min="6" max="1022" width="9" style="2"/>
+    <col min="1023" max="1025" width="11.5703125" style="2" customWidth="1"/>
+    <col min="1026" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="2QGns4GiQXLWp03h1rAnCGwf8C9JX/kwo+ex+hY2Aw/EWWBpXuldjPYc/cc41+/EkF3H6R8gwYt/PrAqDEEvXw==" saltValue="vC+ysnkUc2Mj74tGRrxQlA==" spinCount="100000" sheet="1" objects="1" scenarios="1" insertRows="0" deleteRows="0" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="G5BFD+jG5gtS6osJMgGc0gwpISl141L0qaQGmWOB7iHXIbEhABn3wgUxwY1ggcRrd2AP8Y5NYNQv0TsfwpDTjA==" saltValue="/BZbceeGJzeUyUJD7nFlyw==" spinCount="100000" sheet="1" objects="1" scenarios="1" insertRows="0" deleteRows="0" selectLockedCells="1"/>
   <pageMargins left="0.69930555555555496" right="0.69930555555555496" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>